<commit_message>
Add --lab and --labs options and add --live option
</commit_message>
<xml_diff>
--- a/examples/palabra/lab1/lab1_result.xlsx
+++ b/examples/palabra/lab1/lab1_result.xlsx
@@ -449,12 +449,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>233</t>
+          <t>237</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>166</t>
+          <t>162</t>
         </is>
       </c>
     </row>
@@ -1879,12 +1879,12 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>No answer from `3.0.0.1` to `as1r2`.</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
@@ -1913,12 +1913,12 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>No answer from `3.1.0.1` to `as1r2`.</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
@@ -2066,12 +2066,12 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>No answer from `20.30.0.2` to `as1r2`.</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
@@ -2457,12 +2457,12 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>No answer from `20.30.1.1` to `as2r1`.</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
@@ -7288,7 +7288,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C167"/>
+  <dimension ref="A1:C163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7673,7 +7673,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.1` reachability from device `as1r2`</t>
+          <t>Verifying `3.1.0.2` reachability from device `as1r2`</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -7683,14 +7683,14 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>No answer from `3.0.0.1` to `as1r2`.</t>
+          <t>No answer from `3.1.0.2` to `as1r2`.</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.1` reachability from device `as1r2`</t>
+          <t>Verifying `3.2.0.1` reachability from device `as1r2`</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -7700,14 +7700,14 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>No answer from `3.1.0.1` to `as1r2`.</t>
+          <t>No answer from `3.2.0.1` to `as1r2`.</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.2` reachability from device `as1r2`</t>
+          <t>Verifying `3.2.0.2` reachability from device `as1r2`</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -7717,14 +7717,14 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>No answer from `3.1.0.2` to `as1r2`.</t>
+          <t>No answer from `3.2.0.2` to `as1r2`.</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.1` reachability from device `as1r2`</t>
+          <t>Verifying `1.0.0.2` reachability from device `as2r1`</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -7734,14 +7734,14 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>No answer from `3.2.0.1` to `as1r2`.</t>
+          <t>No answer from `1.0.0.2` to `as2r1`.</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.2` reachability from device `as1r2`</t>
+          <t>Verifying `2.1.0.2` reachability from device `as2r1`</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -7751,14 +7751,14 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>No answer from `3.2.0.2` to `as1r2`.</t>
+          <t>No answer from `2.1.0.2` to `as2r1`.</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.2` reachability from device `as1r2`</t>
+          <t>Verifying `3.1.0.2` reachability from device `as2r1`</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -7768,14 +7768,14 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>No answer from `20.30.0.2` to `as1r2`.</t>
+          <t>No answer from `3.1.0.2` to `as2r1`.</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.2` reachability from device `as2r1`</t>
+          <t>Verifying `3.2.0.1` reachability from device `as2r1`</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -7785,14 +7785,14 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>No answer from `1.0.0.2` to `as2r1`.</t>
+          <t>No answer from `3.2.0.1` to `as2r1`.</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.2` reachability from device `as2r1`</t>
+          <t>Verifying `3.2.0.2` reachability from device `as2r1`</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -7802,14 +7802,14 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>No answer from `2.1.0.2` to `as2r1`.</t>
+          <t>No answer from `3.2.0.2` to `as2r1`.</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.2` reachability from device `as2r1`</t>
+          <t>Verifying `1.0.0.2` reachability from device `as2r2`</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -7819,14 +7819,14 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>No answer from `3.1.0.2` to `as2r1`.</t>
+          <t>No answer from `1.0.0.2` to `as2r2`.</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.1` reachability from device `as2r1`</t>
+          <t>Verifying `2.1.0.2` reachability from device `as2r2`</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -7836,14 +7836,14 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>No answer from `3.2.0.1` to `as2r1`.</t>
+          <t>No answer from `2.1.0.2` to `as2r2`.</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.2` reachability from device `as2r1`</t>
+          <t>Verifying `3.1.0.2` reachability from device `as2r2`</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -7853,14 +7853,14 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>No answer from `3.2.0.2` to `as2r1`.</t>
+          <t>No answer from `3.1.0.2` to `as2r2`.</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.1` reachability from device `as2r1`</t>
+          <t>Verifying `3.2.0.1` reachability from device `as2r2`</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -7870,14 +7870,14 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>No answer from `20.30.1.1` to `as2r1`.</t>
+          <t>No answer from `3.2.0.1` to `as2r2`.</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.2` reachability from device `as2r2`</t>
+          <t>Verifying `3.2.0.2` reachability from device `as2r2`</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -7887,14 +7887,14 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>No answer from `1.0.0.2` to `as2r2`.</t>
+          <t>No answer from `3.2.0.2` to `as2r2`.</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.2` reachability from device `as2r2`</t>
+          <t>Verifying `1.0.0.2` reachability from device `as3r1`</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -7904,14 +7904,14 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>No answer from `2.1.0.2` to `as2r2`.</t>
+          <t>No answer from `1.0.0.2` to `as3r1`.</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.2` reachability from device `as2r2`</t>
+          <t>Verifying `2.1.0.2` reachability from device `as3r1`</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -7921,14 +7921,14 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>No answer from `3.1.0.2` to `as2r2`.</t>
+          <t>No answer from `2.1.0.2` to `as3r1`.</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.1` reachability from device `as2r2`</t>
+          <t>Verifying `3.1.0.2` reachability from device `as3r1`</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -7938,14 +7938,14 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>No answer from `3.2.0.1` to `as2r2`.</t>
+          <t>No answer from `3.1.0.2` to `as3r1`.</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.2` reachability from device `as2r2`</t>
+          <t>Verifying `3.2.0.1` reachability from device `as3r1`</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -7955,14 +7955,14 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>No answer from `3.2.0.2` to `as2r2`.</t>
+          <t>ping: connect: Network is unreachable</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.2` reachability from device `as3r1`</t>
+          <t>Verifying `3.2.0.2` reachability from device `as3r1`</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -7972,14 +7972,14 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>No answer from `1.0.0.2` to `as3r1`.</t>
+          <t>ping: connect: Network is unreachable</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.2` reachability from device `as3r1`</t>
+          <t>Verifying `1.0.0.2` reachability from device `as3r2`</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -7989,14 +7989,14 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>No answer from `2.1.0.2` to `as3r1`.</t>
+          <t>No answer from `1.0.0.2` to `as3r2`.</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.2` reachability from device `as3r1`</t>
+          <t>Verifying `2.1.0.2` reachability from device `as3r2`</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -8006,14 +8006,14 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>No answer from `3.1.0.2` to `as3r1`.</t>
+          <t>No answer from `2.1.0.2` to `as3r2`.</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.1` reachability from device `as3r1`</t>
+          <t>Verifying `3.1.0.2` reachability from device `as3r2`</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -8023,14 +8023,14 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>ping: connect: Network is unreachable</t>
+          <t>No answer from `3.1.0.2` to `as3r2`.</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.2` reachability from device `as3r1`</t>
+          <t>Verifying `3.2.0.1` reachability from device `as3r2`</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -8047,7 +8047,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.2` reachability from device `as3r2`</t>
+          <t>Verifying `3.2.0.2` reachability from device `as3r2`</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -8057,14 +8057,14 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>No answer from `1.0.0.2` to `as3r2`.</t>
+          <t>ping: connect: Network is unreachable</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.2` reachability from device `as3r2`</t>
+          <t>Verifying `1.0.0.1` reachability from device `local`</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -8074,14 +8074,14 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>No answer from `2.1.0.2` to `as3r2`.</t>
+          <t>ping: connect: Network is unreachable</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.2` reachability from device `as3r2`</t>
+          <t>Verifying `1.0.0.2` reachability from device `local`</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -8091,14 +8091,14 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>No answer from `3.1.0.2` to `as3r2`.</t>
+          <t>ping: connect: Network is unreachable</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.1` reachability from device `as3r2`</t>
+          <t>Verifying `1.1.0.1` reachability from device `local`</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -8115,7 +8115,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.2` reachability from device `as3r2`</t>
+          <t>Verifying `1.1.0.2` reachability from device `local`</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -8132,7 +8132,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.1` reachability from device `local`</t>
+          <t>Verifying `2.0.0.1` reachability from device `local`</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -8149,7 +8149,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.2` reachability from device `local`</t>
+          <t>Verifying `2.0.0.2` reachability from device `local`</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -8166,7 +8166,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.1` reachability from device `local`</t>
+          <t>Verifying `2.1.0.1` reachability from device `local`</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -8183,7 +8183,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.2` reachability from device `local`</t>
+          <t>Verifying `2.1.0.2` reachability from device `local`</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -8200,7 +8200,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.1` reachability from device `local`</t>
+          <t>Verifying `3.0.0.1` reachability from device `local`</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -8217,7 +8217,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.2` reachability from device `local`</t>
+          <t>Verifying `3.0.0.2` reachability from device `local`</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -8234,7 +8234,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.1` reachability from device `local`</t>
+          <t>Verifying `3.1.0.1` reachability from device `local`</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -8251,7 +8251,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.2` reachability from device `local`</t>
+          <t>Verifying `3.1.0.2` reachability from device `local`</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -8268,7 +8268,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.1` reachability from device `local`</t>
+          <t>Verifying `3.2.0.1` reachability from device `local`</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -8285,7 +8285,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.2` reachability from device `local`</t>
+          <t>Verifying `3.2.0.2` reachability from device `local`</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -8302,7 +8302,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.1` reachability from device `local`</t>
+          <t>Verifying `10.20.0.1` reachability from device `local`</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -8319,7 +8319,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.2` reachability from device `local`</t>
+          <t>Verifying `10.20.0.2` reachability from device `local`</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -8336,7 +8336,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.1` reachability from device `local`</t>
+          <t>Verifying `10.20.1.1` reachability from device `local`</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -8353,7 +8353,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.2` reachability from device `local`</t>
+          <t>Verifying `10.20.1.2` reachability from device `local`</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -8370,7 +8370,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.1` reachability from device `local`</t>
+          <t>Verifying `20.30.0.1` reachability from device `local`</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -8387,7 +8387,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.2` reachability from device `local`</t>
+          <t>Verifying `20.30.0.2` reachability from device `local`</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -8404,7 +8404,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.1` reachability from device `local`</t>
+          <t>Verifying `20.30.1.1` reachability from device `local`</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -8421,7 +8421,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.2` reachability from device `local`</t>
+          <t>Verifying `20.30.1.2` reachability from device `local`</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -8438,7 +8438,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.1` reachability from device `local`</t>
+          <t>Verifying `1.0.0.1` reachability from device `root`</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -8448,14 +8448,14 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>ping: connect: Network is unreachable</t>
+          <t>Device `root` is not running.</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.2` reachability from device `local`</t>
+          <t>Verifying `1.0.0.2` reachability from device `root`</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -8465,14 +8465,14 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>ping: connect: Network is unreachable</t>
+          <t>Device `root` is not running.</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.1` reachability from device `local`</t>
+          <t>Verifying `1.1.0.1` reachability from device `root`</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -8482,14 +8482,14 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>ping: connect: Network is unreachable</t>
+          <t>Device `root` is not running.</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.2` reachability from device `local`</t>
+          <t>Verifying `1.1.0.2` reachability from device `root`</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -8499,14 +8499,14 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>ping: connect: Network is unreachable</t>
+          <t>Device `root` is not running.</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.1` reachability from device `root`</t>
+          <t>Verifying `2.0.0.1` reachability from device `root`</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -8523,7 +8523,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.2` reachability from device `root`</t>
+          <t>Verifying `2.0.0.2` reachability from device `root`</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -8540,7 +8540,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.1` reachability from device `root`</t>
+          <t>Verifying `2.1.0.1` reachability from device `root`</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -8557,7 +8557,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.2` reachability from device `root`</t>
+          <t>Verifying `2.1.0.2` reachability from device `root`</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -8574,7 +8574,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.1` reachability from device `root`</t>
+          <t>Verifying `3.0.0.1` reachability from device `root`</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -8591,7 +8591,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.2` reachability from device `root`</t>
+          <t>Verifying `3.0.0.2` reachability from device `root`</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -8608,7 +8608,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.1` reachability from device `root`</t>
+          <t>Verifying `3.1.0.1` reachability from device `root`</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -8625,7 +8625,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.2` reachability from device `root`</t>
+          <t>Verifying `3.1.0.2` reachability from device `root`</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -8642,7 +8642,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.1` reachability from device `root`</t>
+          <t>Verifying `3.2.0.1` reachability from device `root`</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -8659,7 +8659,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.2` reachability from device `root`</t>
+          <t>Verifying `3.2.0.2` reachability from device `root`</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -8676,7 +8676,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.1` reachability from device `root`</t>
+          <t>Verifying `10.20.0.1` reachability from device `root`</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -8693,7 +8693,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.2` reachability from device `root`</t>
+          <t>Verifying `10.20.0.2` reachability from device `root`</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -8710,7 +8710,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.1` reachability from device `root`</t>
+          <t>Verifying `10.20.1.1` reachability from device `root`</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -8727,7 +8727,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.2` reachability from device `root`</t>
+          <t>Verifying `10.20.1.2` reachability from device `root`</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -8744,7 +8744,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.1` reachability from device `root`</t>
+          <t>Verifying `20.30.0.1` reachability from device `root`</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -8761,7 +8761,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.2` reachability from device `root`</t>
+          <t>Verifying `20.30.0.2` reachability from device `root`</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -8778,7 +8778,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.1` reachability from device `root`</t>
+          <t>Verifying `20.30.1.1` reachability from device `root`</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -8795,7 +8795,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.2` reachability from device `root`</t>
+          <t>Verifying `20.30.1.2` reachability from device `root`</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -8812,7 +8812,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.1` reachability from device `root`</t>
+          <t>Verifying `1.0.0.1` reachability from device `net`</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -8822,14 +8822,14 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Device `root` is not running.</t>
+          <t>Device `net` is not running.</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.2` reachability from device `root`</t>
+          <t>Verifying `1.0.0.2` reachability from device `net`</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -8839,14 +8839,14 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Device `root` is not running.</t>
+          <t>Device `net` is not running.</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.1` reachability from device `root`</t>
+          <t>Verifying `1.1.0.1` reachability from device `net`</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -8856,14 +8856,14 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Device `root` is not running.</t>
+          <t>Device `net` is not running.</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.2` reachability from device `root`</t>
+          <t>Verifying `1.1.0.2` reachability from device `net`</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -8873,14 +8873,14 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Device `root` is not running.</t>
+          <t>Device `net` is not running.</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.1` reachability from device `net`</t>
+          <t>Verifying `2.0.0.1` reachability from device `net`</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -8897,7 +8897,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.2` reachability from device `net`</t>
+          <t>Verifying `2.0.0.2` reachability from device `net`</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -8914,7 +8914,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.1` reachability from device `net`</t>
+          <t>Verifying `2.1.0.1` reachability from device `net`</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -8931,7 +8931,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.2` reachability from device `net`</t>
+          <t>Verifying `2.1.0.2` reachability from device `net`</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -8948,7 +8948,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.1` reachability from device `net`</t>
+          <t>Verifying `3.0.0.1` reachability from device `net`</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -8965,7 +8965,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.2` reachability from device `net`</t>
+          <t>Verifying `3.0.0.2` reachability from device `net`</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -8982,7 +8982,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.1` reachability from device `net`</t>
+          <t>Verifying `3.1.0.1` reachability from device `net`</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -8999,7 +8999,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.2` reachability from device `net`</t>
+          <t>Verifying `3.1.0.2` reachability from device `net`</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -9016,7 +9016,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.1` reachability from device `net`</t>
+          <t>Verifying `3.2.0.1` reachability from device `net`</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -9033,7 +9033,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.2` reachability from device `net`</t>
+          <t>Verifying `3.2.0.2` reachability from device `net`</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -9050,7 +9050,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.1` reachability from device `net`</t>
+          <t>Verifying `10.20.0.1` reachability from device `net`</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -9067,7 +9067,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.2` reachability from device `net`</t>
+          <t>Verifying `10.20.0.2` reachability from device `net`</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -9084,7 +9084,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.1` reachability from device `net`</t>
+          <t>Verifying `10.20.1.1` reachability from device `net`</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -9101,7 +9101,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.2` reachability from device `net`</t>
+          <t>Verifying `10.20.1.2` reachability from device `net`</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -9118,7 +9118,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.1` reachability from device `net`</t>
+          <t>Verifying `20.30.0.1` reachability from device `net`</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -9135,7 +9135,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.2` reachability from device `net`</t>
+          <t>Verifying `20.30.0.2` reachability from device `net`</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -9152,7 +9152,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.1` reachability from device `net`</t>
+          <t>Verifying `20.30.1.1` reachability from device `net`</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -9169,7 +9169,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.2` reachability from device `net`</t>
+          <t>Verifying `20.30.1.2` reachability from device `net`</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -9186,7 +9186,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.1` reachability from device `net`</t>
+          <t>Verifying `1.1.0.1` reachability from device `pc`</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -9196,14 +9196,14 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Device `net` is not running.</t>
+          <t>ping: connect: Network is unreachable</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.2` reachability from device `net`</t>
+          <t>Verifying `1.1.0.2` reachability from device `pc`</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -9213,14 +9213,14 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Device `net` is not running.</t>
+          <t>ping: connect: Network is unreachable</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.1` reachability from device `net`</t>
+          <t>Verifying `2.0.0.1` reachability from device `pc`</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -9230,14 +9230,14 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Device `net` is not running.</t>
+          <t>ping: connect: Network is unreachable</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.2` reachability from device `net`</t>
+          <t>Verifying `2.0.0.2` reachability from device `pc`</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -9247,14 +9247,14 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Device `net` is not running.</t>
+          <t>ping: connect: Network is unreachable</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.1` reachability from device `pc`</t>
+          <t>Verifying `2.1.0.1` reachability from device `pc`</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -9271,7 +9271,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.2` reachability from device `pc`</t>
+          <t>Verifying `2.1.0.2` reachability from device `pc`</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -9288,7 +9288,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.1` reachability from device `pc`</t>
+          <t>Verifying `3.0.0.1` reachability from device `pc`</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -9305,7 +9305,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.2` reachability from device `pc`</t>
+          <t>Verifying `3.0.0.2` reachability from device `pc`</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -9322,7 +9322,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.1` reachability from device `pc`</t>
+          <t>Verifying `3.1.0.1` reachability from device `pc`</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -9339,7 +9339,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.2` reachability from device `pc`</t>
+          <t>Verifying `3.1.0.2` reachability from device `pc`</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -9356,7 +9356,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.1` reachability from device `pc`</t>
+          <t>Verifying `3.2.0.1` reachability from device `pc`</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -9373,7 +9373,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.2` reachability from device `pc`</t>
+          <t>Verifying `3.2.0.2` reachability from device `pc`</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -9390,7 +9390,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.1` reachability from device `pc`</t>
+          <t>Verifying `10.20.0.1` reachability from device `pc`</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -9407,7 +9407,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.2` reachability from device `pc`</t>
+          <t>Verifying `10.20.0.2` reachability from device `pc`</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -9424,7 +9424,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.1` reachability from device `pc`</t>
+          <t>Verifying `10.20.1.1` reachability from device `pc`</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -9441,7 +9441,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.2` reachability from device `pc`</t>
+          <t>Verifying `10.20.1.2` reachability from device `pc`</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -9458,7 +9458,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.1` reachability from device `pc`</t>
+          <t>Verifying `20.30.0.1` reachability from device `pc`</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -9475,7 +9475,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.2` reachability from device `pc`</t>
+          <t>Verifying `20.30.0.2` reachability from device `pc`</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -9492,7 +9492,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.1` reachability from device `pc`</t>
+          <t>Verifying `20.30.1.1` reachability from device `pc`</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -9509,7 +9509,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.2` reachability from device `pc`</t>
+          <t>Verifying `20.30.1.2` reachability from device `pc`</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -9526,7 +9526,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.1` reachability from device `pc`</t>
+          <t>Checking that named is running on device `net`</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -9536,14 +9536,14 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>ping: connect: Network is unreachable</t>
+          <t>Device net not in the network scenario.</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.2` reachability from device `pc`</t>
+          <t>Checking that watchfrr is not running on device `net`</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -9553,14 +9553,14 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>ping: connect: Network is unreachable</t>
+          <t>Device net not in the network scenario.</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.1` reachability from device `pc`</t>
+          <t>Checking that named is running on device `root`</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -9570,14 +9570,14 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>ping: connect: Network is unreachable</t>
+          <t>Device root not in the network scenario.</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.2` reachability from device `pc`</t>
+          <t>Checking that watchfrr is not running on device `root`</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -9587,14 +9587,14 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>ping: connect: Network is unreachable</t>
+          <t>Device root not in the network scenario.</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Checking that named is running on device `net`</t>
+          <t>as1r1 has bgp peer 1.0.0.2</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -9604,14 +9604,14 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>Device net not in the network scenario.</t>
+          <t>The peering between as1r1 and 1.0.0.2 is not up.</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Checking that watchfrr is not running on device `net`</t>
+          <t>as1r2 has bgp peer 1.0.0.1</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -9621,14 +9621,14 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>Device net not in the network scenario.</t>
+          <t>The peering between as1r2 and 1.0.0.1 is not up.</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Checking that named is running on device `root`</t>
+          <t>Check that route 3.2.0.0/24 IS in the routing table of device `as3r1`</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -9638,14 +9638,14 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>Device root not in the network scenario.</t>
+          <t>The route 3.2.0.0/24 IS NOT found in the routing table of `as3r1`.</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Checking that watchfrr is not running on device `root`</t>
+          <t>Check that route 0.0.0.0/0 IS in the routing table of device `root`</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -9655,14 +9655,14 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Device root not in the network scenario.</t>
+          <t>The route 0.0.0.0/0 IS NOT found in the routing table of `root`.</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>as1r1 has bgp peer 1.0.0.2</t>
+          <t>Check that route 1.1.0.0/24 IS in the routing table of device `root`</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -9672,14 +9672,14 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>The peering between as1r1 and 1.0.0.2 is not up.</t>
+          <t>The route 1.1.0.0/24 IS NOT found in the routing table of `root`.</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>as1r2 has bgp peer 1.0.0.1</t>
+          <t>Check that route 0.0.0.0/0 IS in the routing table of device `net`</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -9689,14 +9689,14 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>The peering between as1r2 and 1.0.0.1 is not up.</t>
+          <t>The route 0.0.0.0/0 IS NOT found in the routing table of `net`.</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Check that route 3.2.0.0/24 IS in the routing table of device `as3r1`</t>
+          <t>Check that route 2.1.0.0/24 IS in the routing table of device `net`</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -9706,14 +9706,14 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>The route 3.2.0.0/24 IS NOT found in the routing table of `as3r1`.</t>
+          <t>The route 2.1.0.0/24 IS NOT found in the routing table of `net`.</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Check that route 0.0.0.0/0 IS in the routing table of device `root`</t>
+          <t>Check that route 0.0.0.0/0 IS in the routing table of device `pc`</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -9723,14 +9723,14 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>The route 0.0.0.0/0 IS NOT found in the routing table of `root`.</t>
+          <t>The route 0.0.0.0/0 IS NOT found in the routing table of `pc`.</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Check that route 1.1.0.0/24 IS in the routing table of device `root`</t>
+          <t>Check that route 3.1.0.0/24 IS in the routing table of device `pc`</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -9740,14 +9740,14 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>The route 1.1.0.0/24 IS NOT found in the routing table of `root`.</t>
+          <t>The route 3.1.0.0/24 IS NOT found in the routing table of `pc`.</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Check that route 0.0.0.0/0 IS in the routing table of device `net`</t>
+          <t>Check that route 0.0.0.0/0 IS in the routing table of device `local`</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
@@ -9757,14 +9757,14 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>The route 0.0.0.0/0 IS NOT found in the routing table of `net`.</t>
+          <t>The route 0.0.0.0/0 IS NOT found in the routing table of `local`.</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Check that route 2.1.0.0/24 IS in the routing table of device `net`</t>
+          <t>Check that route 3.2.0.0/24 IS in the routing table of device `local`</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -9774,14 +9774,14 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>The route 2.1.0.0/24 IS NOT found in the routing table of `net`.</t>
+          <t>The route 3.2.0.0/24 IS NOT found in the routing table of `local`.</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Check that route 0.0.0.0/0 IS in the routing table of device `pc`</t>
+          <t>Checking on `root` that `1.1.0.2` is the authority for domain `.`</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -9791,14 +9791,14 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>The route 0.0.0.0/0 IS NOT found in the routing table of `pc`.</t>
+          <t>Device `root` is not running.</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Check that route 3.1.0.0/24 IS in the routing table of device `pc`</t>
+          <t>Checking on `root` that `1.1.0.2` is the authority for domain `.`</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -9808,14 +9808,14 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>The route 3.1.0.0/24 IS NOT found in the routing table of `pc`.</t>
+          <t>Device `root` is not running.</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Check that route 0.0.0.0/0 IS in the routing table of device `local`</t>
+          <t>Checking on `local` that `1.1.0.2` is the authority for domain `.`</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
@@ -9825,14 +9825,14 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>The route 0.0.0.0/0 IS NOT found in the routing table of `local`.</t>
+          <t>named on local is running but answered with REFUSED when quering for .</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Check that route 3.2.0.0/24 IS in the routing table of device `local`</t>
+          <t>Checking on `net` that `2.1.0.2` is the authority for domain `net`</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
@@ -9842,14 +9842,14 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>The route 3.2.0.0/24 IS NOT found in the routing table of `local`.</t>
+          <t>Device `net` is not running.</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>Checking on `root` that `1.1.0.2` is the authority for domain `.`</t>
+          <t>Checking that `3.2.0.2` is the local name server for device `as1r1`</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -9859,14 +9859,14 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>Device `root` is not running.</t>
+          <t>`resolv.conf` file not found for device `as1r1`</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>Checking on `root` that `1.1.0.2` is the authority for domain `.`</t>
+          <t>Checking that `3.2.0.2` is the local name server for device `as1r2`</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -9876,14 +9876,14 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>Device `root` is not running.</t>
+          <t>`resolv.conf` file not found for device `as1r2`</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>Checking on `local` that `1.1.0.2` is the authority for domain `.`</t>
+          <t>Checking that `3.2.0.2` is the local name server for device `as2r1`</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -9893,14 +9893,14 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>named on local is running but answered with REFUSED when quering for .</t>
+          <t>`resolv.conf` file not found for device `as2r1`</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>Checking on `net` that `2.1.0.2` is the authority for domain `net`</t>
+          <t>Checking that `3.2.0.2` is the local name server for device `as2r2`</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -9910,14 +9910,14 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>Device `net` is not running.</t>
+          <t>`resolv.conf` file not found for device `as2r2`</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>Checking that `3.2.0.2` is the local name server for device `as1r1`</t>
+          <t>Checking that `3.2.0.2` is the local name server for device `as3r1`</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
@@ -9927,14 +9927,14 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>`resolv.conf` file not found for device `as1r1`</t>
+          <t>`resolv.conf` file not found for device `as3r1`</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>Checking that `3.2.0.2` is the local name server for device `as1r2`</t>
+          <t>Checking that `3.2.0.2` is the local name server for device `as3r2`</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
@@ -9944,14 +9944,14 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>`resolv.conf` file not found for device `as1r2`</t>
+          <t>`resolv.conf` file not found for device `as3r2`</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>Checking that `3.2.0.2` is the local name server for device `as2r1`</t>
+          <t>Checking that `3.2.0.2` is the local name server for device `pc`</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
@@ -9961,14 +9961,14 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>`resolv.conf` file not found for device `as2r1`</t>
+          <t>The local name server for device `pc` has ip `3.2.0.2`</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>Checking that `3.2.0.2` is the local name server for device `as2r2`</t>
+          <t>Verifying `pc.net` reachability from device `as1r1`</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
@@ -9978,14 +9978,14 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>`resolv.conf` file not found for device `as2r2`</t>
+          <t>ping: pc.net: Temporary failure in name resolution</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>Checking that `3.2.0.2` is the local name server for device `as3r1`</t>
+          <t>Verifying `pc.net` reachability from device `as1r2`</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
@@ -9995,14 +9995,14 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>`resolv.conf` file not found for device `as3r1`</t>
+          <t>ping: pc.net: Temporary failure in name resolution</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>Checking that `3.2.0.2` is the local name server for device `as3r2`</t>
+          <t>Verifying `pc.net` reachability from device `as2r1`</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -10012,14 +10012,14 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>`resolv.conf` file not found for device `as3r2`</t>
+          <t>ping: pc.net: Temporary failure in name resolution</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>Checking that `3.2.0.2` is the local name server for device `pc`</t>
+          <t>Verifying `pc.net` reachability from device `as2r2`</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -10029,14 +10029,14 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>The local name server for device `pc` has ip `3.2.0.2`</t>
+          <t>ping: pc.net: Temporary failure in name resolution</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>Verifying `pc.net` reachability from device `as1r1`</t>
+          <t>Verifying `pc.net` reachability from device `as3r1`</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -10053,7 +10053,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>Verifying `pc.net` reachability from device `as1r2`</t>
+          <t>Verifying `pc.net` reachability from device `as3r2`</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
@@ -10062,74 +10062,6 @@
         </is>
       </c>
       <c r="C163" t="inlineStr">
-        <is>
-          <t>ping: pc.net: Temporary failure in name resolution</t>
-        </is>
-      </c>
-    </row>
-    <row r="164">
-      <c r="A164" t="inlineStr">
-        <is>
-          <t>Verifying `pc.net` reachability from device `as2r1`</t>
-        </is>
-      </c>
-      <c r="B164" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="C164" t="inlineStr">
-        <is>
-          <t>ping: pc.net: Temporary failure in name resolution</t>
-        </is>
-      </c>
-    </row>
-    <row r="165">
-      <c r="A165" t="inlineStr">
-        <is>
-          <t>Verifying `pc.net` reachability from device `as2r2`</t>
-        </is>
-      </c>
-      <c r="B165" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="C165" t="inlineStr">
-        <is>
-          <t>ping: pc.net: Temporary failure in name resolution</t>
-        </is>
-      </c>
-    </row>
-    <row r="166">
-      <c r="A166" t="inlineStr">
-        <is>
-          <t>Verifying `pc.net` reachability from device `as3r1`</t>
-        </is>
-      </c>
-      <c r="B166" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="C166" t="inlineStr">
-        <is>
-          <t>ping: pc.net: Temporary failure in name resolution</t>
-        </is>
-      </c>
-    </row>
-    <row r="167">
-      <c r="A167" t="inlineStr">
-        <is>
-          <t>Verifying `pc.net` reachability from device `as3r2`</t>
-        </is>
-      </c>
-      <c r="B167" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="C167" t="inlineStr">
         <is>
           <t>ping: pc.net: Temporary failure in name resolution</t>
         </is>

</xml_diff>